<commit_message>
New Schematic for Rev 3 and updated BOM
</commit_message>
<xml_diff>
--- a/Bill Of Materials/Bill of Materials.xlsx
+++ b/Bill Of Materials/Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ECE-411-Practicum\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8738AC0-C383-436F-8F21-7F1319B05488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE9E45-79C7-491C-942C-95799225BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
   <si>
     <t>Count</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Bill of Materials for: TEAM 3, Color Sensor Pen</t>
   </si>
   <si>
-    <t>BOM Version: 1.0</t>
-  </si>
-  <si>
     <t>P/NP = Place/ Not Place (on PCB board)</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>J4</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -97,12 +88,6 @@
   </si>
   <si>
     <t>SW1</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>TP1, TP2, TP3, TP4</t>
   </si>
   <si>
     <t>U1</t>
@@ -127,9 +112,6 @@
 0.1 µF ±10% 50V Ceramic Capacitor X7R 1206 (3216 Metric)</t>
   </si>
   <si>
-    <t>20 pF ±5% 50V Ceramic Capacitor C0G, NP0 1206 (3216 Metric)</t>
-  </si>
-  <si>
     <t>1276-3086-1-ND</t>
   </si>
   <si>
@@ -160,12 +142,6 @@
     <t>CL31B104KBCNFNC</t>
   </si>
   <si>
-    <t>CC1206JRNPO9BN200</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
@@ -223,9 +199,6 @@
     <t>1276-2744-1-ND</t>
   </si>
   <si>
-    <t>311-1153-1-ND</t>
-  </si>
-  <si>
     <t>I2C Display Module 0.91 Inch Resolution: 128 x 32 3.3V~5V</t>
   </si>
   <si>
@@ -265,9 +238,6 @@
     <t>835-RT9078-33GJ5</t>
   </si>
   <si>
-    <t>J5 (Alternative)</t>
-  </si>
-  <si>
     <t>U1 (Alternative)</t>
   </si>
   <si>
@@ -307,9 +277,18 @@
     <t>160-2182-1-ND</t>
   </si>
   <si>
+    <t>Slide Switch DPDT Through Hole</t>
+  </si>
+  <si>
+    <t>JS202011CQN</t>
+  </si>
+  <si>
     <t>C&amp;K</t>
   </si>
   <si>
+    <t>401-2001-ND</t>
+  </si>
+  <si>
     <t>D6R90 F1 LFS</t>
   </si>
   <si>
@@ -340,21 +319,9 @@
     <t>Oupiin</t>
   </si>
   <si>
-    <t>1X7 Connector Header Through Hole 7 position 0.100" (2.54mm)</t>
-  </si>
-  <si>
-    <t>2011-1X07G00SB</t>
-  </si>
-  <si>
-    <t>2553-2011-1X07G00SB-ND</t>
-  </si>
-  <si>
     <t>2553-2011-1X08TSB-ND</t>
   </si>
   <si>
-    <t>1X6 Connector Header Through Hole 8 position 0.100" (2.54mm)</t>
-  </si>
-  <si>
     <t>1X4 Connector Header Through Hole 8 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -376,28 +343,46 @@
     <t>Battery Storage Box Case Holder for 18650</t>
   </si>
   <si>
-    <t>2223-TS02-66-60-BK-100-SCR-D-ND</t>
-  </si>
-  <si>
-    <t>Tactile Switch SPST-NO Top Actuated Through Hole</t>
-  </si>
-  <si>
-    <t>TS02-66-60-BK-100-SCR-D</t>
-  </si>
-  <si>
-    <t>Last Modified 11/8/2023</t>
-  </si>
-  <si>
-    <t>PCB Rev: 2.0</t>
-  </si>
-  <si>
-    <t>JS202011CQN</t>
-  </si>
-  <si>
-    <t>401-2001-ND</t>
-  </si>
-  <si>
-    <t>Slide Switch DPDT Through Hole</t>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>10 pF ±5% 10V Ceramic Capacitor C0G, NP0 1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>885012008001</t>
+  </si>
+  <si>
+    <t>732-7861-1-ND</t>
+  </si>
+  <si>
+    <t>1X3 Connector Header Through Hole 8 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>PCB Rev: 3.0</t>
+  </si>
+  <si>
+    <t>BOM Version: 3.0</t>
+  </si>
+  <si>
+    <t>VR1</t>
+  </si>
+  <si>
+    <t>VR1 (Alternative)</t>
+  </si>
+  <si>
+    <t>Note: only need to buy 1 for both J3 and J4</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3</t>
+  </si>
+  <si>
+    <t>Last Modified 11/10/2023</t>
   </si>
 </sst>
 </file>
@@ -494,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -527,6 +512,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -543,6 +529,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -842,23 +832,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C6AA7B-3CE6-4102-AAB7-095645F7575D}">
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
     <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="85.109375" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" style="11" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" style="9" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="6" customWidth="1"/>
@@ -874,20 +864,20 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -904,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>4</v>
@@ -916,10 +906,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="7"/>
@@ -931,32 +921,32 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
+        <v>105</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="I6" s="11">
-        <v>0.25</v>
+        <v>0.11</v>
       </c>
       <c r="J6" s="9">
         <f xml:space="preserve"> I6*A6</f>
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -964,31 +954,31 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I7" s="11">
         <v>0.11</v>
       </c>
       <c r="J7" s="9">
-        <f t="shared" ref="J7:J29" si="0" xml:space="preserve"> I7*A7</f>
+        <f t="shared" ref="J7:J11" si="0" xml:space="preserve"> I7*A7</f>
         <v>0.33</v>
       </c>
     </row>
@@ -997,25 +987,25 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I8" s="11">
         <v>0.13</v>
@@ -1030,25 +1020,25 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I9" s="11">
         <v>0.41</v>
@@ -1063,25 +1053,25 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I10" s="11">
         <v>0.13</v>
@@ -1096,25 +1086,25 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I11" s="11">
         <v>0.08</v>
@@ -1129,32 +1119,35 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I12" s="11">
         <v>0.08</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I13*A13</f>
         <v>0.08</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1162,32 +1155,28 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="I13" s="11">
-        <v>0.38</v>
-      </c>
-      <c r="J13" s="9">
-        <f xml:space="preserve"> I13*A13</f>
-        <v>0.38</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1195,28 +1184,32 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="I14" s="11">
-        <v>0.36</v>
+        <v>0.38</v>
+      </c>
+      <c r="J14" s="9">
+        <f xml:space="preserve"> I14*A14</f>
+        <v>0.38</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1224,32 +1217,28 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="I15" s="11">
-        <v>0.08</v>
-      </c>
-      <c r="J15" s="9">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1257,31 +1246,31 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I16" s="11">
         <v>0.24</v>
       </c>
       <c r="J16" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I16*A16</f>
         <v>0.24</v>
       </c>
     </row>
@@ -1290,31 +1279,31 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I17" s="11">
         <v>0.1</v>
       </c>
       <c r="J17" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I17*A17</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -1323,31 +1312,31 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I18" s="11">
         <v>0.1</v>
       </c>
       <c r="J18" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I18*A18</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -1356,32 +1345,32 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="I19" s="11">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="J19" s="9">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f xml:space="preserve"> I19*A19</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1389,31 +1378,31 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I20" s="11">
         <v>1.1200000000000001</v>
       </c>
       <c r="J20" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I20*A20</f>
         <v>1.1200000000000001</v>
       </c>
     </row>
@@ -1422,28 +1411,28 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I21" s="11">
         <v>0</v>
       </c>
       <c r="J21" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I21*A21</f>
         <v>0</v>
       </c>
     </row>
@@ -1452,31 +1441,31 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I22" s="11">
         <v>3.03</v>
       </c>
       <c r="J22" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I22*A22</f>
         <v>3.03</v>
       </c>
     </row>
@@ -1485,25 +1474,25 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I23" s="11">
         <v>1.74</v>
@@ -1514,31 +1503,31 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I24" s="11">
         <v>0.26</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I24*A24</f>
         <v>0.26</v>
       </c>
     </row>
@@ -1547,28 +1536,28 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I25" s="11">
         <v>2.7890000000000001</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I25*A25</f>
         <v>2.7890000000000001</v>
       </c>
     </row>
@@ -1577,28 +1566,28 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
         <v>59</v>
       </c>
-      <c r="D26" t="s">
-        <v>68</v>
-      </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I26" s="11">
         <v>6.95</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I26*A26</f>
         <v>6.95</v>
       </c>
     </row>
@@ -1607,28 +1596,28 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="I27" s="11">
         <v>3.66</v>
       </c>
       <c r="J27" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I27*A27</f>
         <v>3.66</v>
       </c>
     </row>
@@ -1637,28 +1626,28 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="I28" s="11">
         <v>0.77900000000000003</v>
       </c>
       <c r="J28" s="9">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> I28*A28</f>
         <v>0.77900000000000003</v>
       </c>
     </row>
@@ -1667,22 +1656,22 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G29" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="I29" s="11">
         <v>0.83625000000000005</v>
@@ -1692,54 +1681,23 @@
         <v>0.83625000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" t="s">
-        <v>121</v>
-      </c>
-      <c r="F30" t="s">
-        <v>123</v>
-      </c>
-      <c r="G30" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="J30" s="9">
-        <f xml:space="preserve"> I30*A30</f>
-        <v>0.6</v>
-      </c>
-    </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I31" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J31" s="9">
         <f>SUM(J6:J29)</f>
-        <v>22.614249999999998</v>
-      </c>
-    </row>
-    <row r="1048576" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J1048576" s="9">
-        <f>SUM(J1:J1048575)</f>
-        <v>45.828499999999998</v>
+        <v>22.754249999999999</v>
+      </c>
+    </row>
+    <row r="1048575" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J1048575" s="9">
+        <f>SUM(J1:J1048574)</f>
+        <v>45.508499999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rev4 Fixed Footprint and Schematic Layout a bit.
Monday 11/13/2023 Will do the PCB final routing
</commit_message>
<xml_diff>
--- a/Bill Of Materials/Bill of Materials.xlsx
+++ b/Bill Of Materials/Bill of Materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ECE-411-Practicum\Bill Of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88543b8e3d642bd/School One Drive/ECE 2023/ECE 411 Industry Design Process/Github ECE 411/ECE-411-Practicum/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE9E45-79C7-491C-942C-95799225BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{93FE9E45-79C7-491C-942C-95799225BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AEE4F53-B9D4-4E65-82CF-F20715221BA9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
+    <workbookView xWindow="660" yWindow="3885" windowWidth="24495" windowHeight="15345" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -529,10 +540,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -836,43 +843,43 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -880,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -916,7 +923,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -949,7 +956,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -982,7 +989,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1048,7 +1055,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1081,7 +1088,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1241,7 +1248,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1270,11 +1277,11 @@
         <v>0.24</v>
       </c>
       <c r="J16" s="9">
-        <f xml:space="preserve"> I16*A16</f>
+        <f t="shared" ref="J16:J22" si="1" xml:space="preserve"> I16*A16</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1303,11 +1310,11 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="9">
-        <f xml:space="preserve"> I17*A17</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1336,11 +1343,11 @@
         <v>0.1</v>
       </c>
       <c r="J18" s="9">
-        <f xml:space="preserve"> I18*A18</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1369,11 +1376,11 @@
         <v>0.6</v>
       </c>
       <c r="J19" s="9">
-        <f xml:space="preserve"> I19*A19</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1402,11 +1409,11 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J20" s="9">
-        <f xml:space="preserve"> I20*A20</f>
+        <f t="shared" si="1"/>
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1432,11 +1439,11 @@
         <v>0</v>
       </c>
       <c r="J21" s="9">
-        <f xml:space="preserve"> I21*A21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1465,11 +1472,11 @@
         <v>3.03</v>
       </c>
       <c r="J22" s="9">
-        <f xml:space="preserve"> I22*A22</f>
+        <f t="shared" si="1"/>
         <v>3.03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1498,7 +1505,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1527,11 +1534,11 @@
         <v>0.26</v>
       </c>
       <c r="J24" s="9">
-        <f xml:space="preserve"> I24*A24</f>
+        <f t="shared" ref="J24:J29" si="2" xml:space="preserve"> I24*A24</f>
         <v>0.26</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1557,11 +1564,11 @@
         <v>2.7890000000000001</v>
       </c>
       <c r="J25" s="9">
-        <f xml:space="preserve"> I25*A25</f>
+        <f t="shared" si="2"/>
         <v>2.7890000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1587,11 +1594,11 @@
         <v>6.95</v>
       </c>
       <c r="J26" s="9">
-        <f xml:space="preserve"> I26*A26</f>
+        <f t="shared" si="2"/>
         <v>6.95</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1617,11 +1624,11 @@
         <v>3.66</v>
       </c>
       <c r="J27" s="9">
-        <f xml:space="preserve"> I27*A27</f>
+        <f t="shared" si="2"/>
         <v>3.66</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1647,11 +1654,11 @@
         <v>0.77900000000000003</v>
       </c>
       <c r="J28" s="9">
-        <f xml:space="preserve"> I28*A28</f>
+        <f t="shared" si="2"/>
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1677,11 +1684,11 @@
         <v>0.83625000000000005</v>
       </c>
       <c r="J29" s="9">
-        <f xml:space="preserve"> I29*A29</f>
+        <f t="shared" si="2"/>
         <v>0.83625000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I31" s="13" t="s">
         <v>95</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>22.754249999999999</v>
       </c>
     </row>
-    <row r="1048575" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="1048575" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J1048575" s="9">
         <f>SUM(J1:J1048574)</f>
         <v>45.508499999999998</v>

</xml_diff>

<commit_message>
update BOM and real capacitor value for crystal
</commit_message>
<xml_diff>
--- a/Bill Of Materials/Bill of Materials.xlsx
+++ b/Bill Of Materials/Bill of Materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a88543b8e3d642bd/School One Drive/ECE 2023/ECE 411 Industry Design Process/Github ECE 411/ECE-411-Practicum/Bill Of Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ECE-411-Practicum\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{93FE9E45-79C7-491C-942C-95799225BD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AEE4F53-B9D4-4E65-82CF-F20715221BA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3E05A7-CB86-4453-86F2-74E50D5A35B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="3885" windowWidth="24495" windowHeight="15345" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D402E5DD-C41C-43D4-B0E5-F14B0B5BA4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="126">
   <si>
     <t>Count</t>
   </si>
@@ -105,9 +94,6 @@
   </si>
   <si>
     <t>Y1</t>
-  </si>
-  <si>
-    <t>SW_MEC_5E</t>
   </si>
   <si>
     <t>TestPoint</t>
@@ -354,18 +340,6 @@
     <t>Battery Storage Box Case Holder for 18650</t>
   </si>
   <si>
-    <t>Würth Elektronik</t>
-  </si>
-  <si>
-    <t>10 pF ±5% 10V Ceramic Capacitor C0G, NP0 1206 (3216 Metric)</t>
-  </si>
-  <si>
-    <t>885012008001</t>
-  </si>
-  <si>
-    <t>732-7861-1-ND</t>
-  </si>
-  <si>
     <t>1X3 Connector Header Through Hole 8 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -375,25 +349,61 @@
     <t>SW2</t>
   </si>
   <si>
-    <t>PCB Rev: 3.0</t>
-  </si>
-  <si>
-    <t>BOM Version: 3.0</t>
-  </si>
-  <si>
-    <t>VR1</t>
-  </si>
-  <si>
-    <t>VR1 (Alternative)</t>
-  </si>
-  <si>
     <t>Note: only need to buy 1 for both J3 and J4</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3</t>
-  </si>
-  <si>
     <t>Last Modified 11/10/2023</t>
+  </si>
+  <si>
+    <t>43 pF ±5% 50V Ceramic Capacitor C0G, NP0 1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>C1206C430J5GAC7800</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>399-14687-1-ND</t>
+  </si>
+  <si>
+    <t>Tactile Switch SPST-NO Top Actuated Through Hole</t>
+  </si>
+  <si>
+    <t>TS02-66-60-BK-100-SCR-D</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>2223-TS02-66-60-BK-100-SCR-D-ND</t>
+  </si>
+  <si>
+    <t>Pushbutton Switch SPST-NO Keyswitch Through Hole</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>TP1-T8</t>
+  </si>
+  <si>
+    <t>PCB Rev: 4.0</t>
+  </si>
+  <si>
+    <t>BOM Version: 4.0</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U2 (Alternative)</t>
+  </si>
+  <si>
+    <t>1X5 Connector Header Through Hole 8 position 0.100" (2.54mm)</t>
   </si>
 </sst>
 </file>
@@ -839,55 +849,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C6AA7B-3CE6-4102-AAB7-095645F7575D}">
-  <dimension ref="A1:N1048575"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="87.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -913,17 +923,17 @@
         <v>6</v>
       </c>
       <c r="I5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="7"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -931,32 +941,32 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I6" s="11">
-        <v>0.11</v>
+        <v>0.39</v>
       </c>
       <c r="J6" s="9">
         <f xml:space="preserve"> I6*A6</f>
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -964,22 +974,22 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="11">
         <v>0.11</v>
@@ -989,7 +999,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -997,22 +1007,22 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="11">
         <v>0.13</v>
@@ -1022,7 +1032,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1030,22 +1040,22 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
         <v>81</v>
-      </c>
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>82</v>
       </c>
       <c r="I9" s="11">
         <v>0.41</v>
@@ -1055,7 +1065,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1063,22 +1073,22 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
         <v>91</v>
       </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" s="11">
         <v>0.13</v>
@@ -1088,7 +1098,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1096,22 +1106,22 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
         <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>97</v>
       </c>
       <c r="I11" s="11">
         <v>0.08</v>
@@ -1121,30 +1131,30 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
         <v>96</v>
-      </c>
-      <c r="E12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" t="s">
-        <v>97</v>
       </c>
       <c r="I12" s="11">
         <v>0.08</v>
@@ -1154,10 +1164,10 @@
         <v>0.08</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1165,51 +1175,51 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
         <v>96</v>
-      </c>
-      <c r="E13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" t="s">
-        <v>97</v>
       </c>
       <c r="I13" s="11">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
       </c>
       <c r="I14" s="11">
         <v>0.38</v>
@@ -1219,36 +1229,36 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
         <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" t="s">
-        <v>69</v>
       </c>
       <c r="I15" s="11">
         <v>0.36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1256,32 +1266,32 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
         <v>76</v>
-      </c>
-      <c r="G16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" t="s">
-        <v>77</v>
       </c>
       <c r="I16" s="11">
         <v>0.24</v>
       </c>
       <c r="J16" s="9">
-        <f t="shared" ref="J16:J22" si="1" xml:space="preserve"> I16*A16</f>
+        <f t="shared" ref="J16:J24" si="1" xml:space="preserve"> I16*A16</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1289,22 +1299,22 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I17" s="11">
         <v>0.1</v>
@@ -1314,7 +1324,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1322,22 +1332,22 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" t="s">
         <v>31</v>
-      </c>
-      <c r="G18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" t="s">
-        <v>32</v>
       </c>
       <c r="I18" s="11">
         <v>0.1</v>
@@ -1347,7 +1357,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1355,352 +1365,412 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="I19" s="11">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="J19" s="9">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> I19*A20</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
       <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="J20" s="9">
+        <f xml:space="preserve"> I20*A20</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
         <v>85</v>
       </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="I21" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="J21" s="9">
+        <f xml:space="preserve"> I21*A21</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="J22" s="9">
+        <f xml:space="preserve"> I22*A22</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
         <v>23</v>
       </c>
-      <c r="G20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" t="s">
-        <v>88</v>
-      </c>
-      <c r="I20" s="11">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="J20" s="9">
-        <f t="shared" si="1"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="11">
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="11">
         <v>0</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J23" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
         <v>43</v>
       </c>
-      <c r="E22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G24" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="11">
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="11">
         <v>3.03</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J24" s="9">
         <f t="shared" si="1"/>
         <v>3.03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
         <v>52</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I25" s="11">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="J26" s="9">
+        <f t="shared" ref="J26:J31" si="2" xml:space="preserve"> I26*A26</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="G23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="11">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="11">
-        <v>0.26</v>
-      </c>
-      <c r="J24" s="9">
-        <f t="shared" ref="J24:J29" si="2" xml:space="preserve"> I24*A24</f>
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" t="s">
-        <v>93</v>
-      </c>
-      <c r="I25" s="11">
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="11">
         <v>2.7890000000000001</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J27" s="9">
         <f t="shared" si="2"/>
         <v>2.7890000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" t="s">
         <v>59</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
         <v>60</v>
       </c>
-      <c r="F26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" s="11">
+      <c r="I28" s="11">
         <v>6.95</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J28" s="9">
         <f t="shared" si="2"/>
         <v>6.95</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
         <v>73</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" t="s">
         <v>74</v>
       </c>
-      <c r="F27" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" t="s">
-        <v>75</v>
-      </c>
-      <c r="I27" s="11">
+      <c r="I29" s="11">
         <v>3.66</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J29" s="9">
         <f t="shared" si="2"/>
         <v>3.66</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
         <v>100</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" t="s">
         <v>101</v>
       </c>
-      <c r="F28" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="11">
+      <c r="I30" s="11">
         <v>0.77900000000000003</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J30" s="9">
         <f t="shared" si="2"/>
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
         <v>103</v>
       </c>
-      <c r="I29" s="11">
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="11">
         <v>0.83625000000000005</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J31" s="9">
         <f t="shared" si="2"/>
         <v>0.83625000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="9">
-        <f>SUM(J6:J29)</f>
-        <v>22.754249999999999</v>
-      </c>
-    </row>
-    <row r="1048575" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J1048575" s="9">
-        <f>SUM(J1:J1048574)</f>
-        <v>45.508499999999998</v>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I33" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" s="9">
+        <f>SUM(J6:J31)</f>
+        <v>24.334250000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>